<commit_message>
UI update David ILunga
</commit_message>
<xml_diff>
--- a/sommatif3/AutreDoc/Registre Canabis.xlsx
+++ b/sommatif3/AutreDoc/Registre Canabis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\myLab\sommatif3_V3 1\sommatif3_V3\sommatif3_V3\sommatif3\sommatif3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\laCite\session4\projet integration\sommatif3 3\sommatif3\sommatif3\AutreDoc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FBBB2B4B-6258-40D2-9113-685CBC254066}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{338C146C-12D9-4226-90DE-AE2903C9C576}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{633A98CD-2610-4587-8EC1-175615D0DA30}"/>
+    <workbookView xWindow="1815" yWindow="1815" windowWidth="21600" windowHeight="11295" xr2:uid="{633A98CD-2610-4587-8EC1-175615D0DA30}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -170,7 +170,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
   <si>
     <t>Etat de santé</t>
   </si>
@@ -242,9 +242,6 @@
   </si>
   <si>
     <t>Space Cake</t>
-  </si>
-  <si>
-    <t>Menu déroulant:</t>
   </si>
   <si>
     <t>initiation</t>
@@ -269,7 +266,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -284,12 +281,6 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -747,8 +738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F55D6410-49A1-4F36-8A56-93C5182D0AEE}">
   <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -821,19 +812,19 @@
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H2">
         <v>1</v>
       </c>
       <c r="I2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K2" t="s">
         <v>29</v>
-      </c>
-      <c r="K2" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -853,19 +844,19 @@
         <v>21</v>
       </c>
       <c r="F3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H3">
         <v>1</v>
       </c>
       <c r="I3" t="s">
+        <v>28</v>
+      </c>
+      <c r="K3" t="s">
         <v>29</v>
-      </c>
-      <c r="K3" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -885,19 +876,19 @@
         <v>22</v>
       </c>
       <c r="F4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H4">
         <v>1</v>
       </c>
       <c r="I4" t="s">
+        <v>28</v>
+      </c>
+      <c r="K4" t="s">
         <v>29</v>
-      </c>
-      <c r="K4" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -917,19 +908,19 @@
         <v>23</v>
       </c>
       <c r="F5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" t="s">
         <v>27</v>
-      </c>
-      <c r="G5" t="s">
-        <v>28</v>
       </c>
       <c r="H5">
         <v>0</v>
       </c>
       <c r="I5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K5" t="s">
         <v>29</v>
-      </c>
-      <c r="K5" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>